<commit_message>
DRTII-601 updating LGW excel upload column names
</commit_message>
<xml_diff>
--- a/server/src/test/resources/LGW_Forecast_Fixture.xlsx
+++ b/server/src/test/resources/LGW_Forecast_Fixture.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilesh/HO_DRT/drt-v2/server/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B10493-789D-5E43-A842-47E2871921FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7939B79A-6D30-514E-A439-A79402FB5AA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15900" xr2:uid="{0663B09F-C0D7-4686-ACD9-8FF02FAE6961}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>OpeFlightNo</t>
-  </si>
-  <si>
     <t>Service</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
     <t>Known Op</t>
   </si>
   <si>
-    <t>Sum of Pax</t>
-  </si>
-  <si>
     <t>Passenger</t>
   </si>
   <si>
@@ -126,6 +120,12 @@
   </si>
   <si>
     <t>TST005</t>
+  </si>
+  <si>
+    <t>FlightNo</t>
+  </si>
+  <si>
+    <t>Forecast Pax</t>
   </si>
 </sst>
 </file>
@@ -647,7 +647,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -656,8 +656,8 @@
     <col min="2" max="6" width="12.33203125" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" customWidth="1"/>
-    <col min="9" max="9" width="6.83203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9" style="2"/>
+    <col min="9" max="9" width="12.5" style="2" customWidth="1"/>
+    <col min="10" max="10" width="14" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.15">
@@ -665,31 +665,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>4</v>
-      </c>
       <c r="I1" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -700,25 +700,25 @@
         <v>0.20833333333333334</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G2" s="4">
         <v>320</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J2" s="7">
         <v>94.569617486338814</v>
@@ -732,25 +732,25 @@
         <v>0.2986111111111111</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="I3" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="J3" s="7">
         <v>54.166666666666671</v>
@@ -764,25 +764,25 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G4" s="4">
         <v>320</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J4" s="7">
         <v>0</v>
@@ -796,25 +796,25 @@
         <v>0.33680555555555558</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G5" s="4">
         <v>319</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J5" s="7">
         <v>0</v>
@@ -828,25 +828,25 @@
         <v>0.31944444444444448</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G6" s="4">
         <v>223</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J6" s="7">
         <v>14.500000000000009</v>

</xml_diff>

<commit_message>
DRTII-726 parsing valid data and ignore invalid data
</commit_message>
<xml_diff>
--- a/server/src/test/resources/LGW_Forecast_Fixture.xlsx
+++ b/server/src/test/resources/LGW_Forecast_Fixture.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilesh/HO_DRT/drt-v2/server/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7939B79A-6D30-514E-A439-A79402FB5AA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4781631D-DC72-0048-A04C-C6A405FCF381}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15900" xr2:uid="{0663B09F-C0D7-4686-ACD9-8FF02FAE6961}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -644,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF66ACCD-9152-4728-B435-3305158BCCDE}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -852,6 +852,34 @@
         <v>14.500000000000009</v>
       </c>
     </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A7" s="8">
+        <v>44022</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="4">
+        <v>223</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="7">
+        <v>14.500000000000009</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>